<commit_message>
doc: update routes table
</commit_message>
<xml_diff>
--- a/doc/Sprint 1/routes table/routes_table.xlsx
+++ b/doc/Sprint 1/routes table/routes_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads_idm\Compressed\Skripsi_fathan - Copy\Skripsi Latex\Diagram\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andri\Desktop\FishCulture\doc\Sprint 1\routes table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D64CA368-7F48-4592-B388-2FDD5F9499DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843DDFBD-239F-4121-831C-28AAB130E2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C254AC1B-B4CF-49CB-B06F-3FDC00B6733D}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>menambahkan / mendaftarkan kolam</t>
   </si>
   <si>
-    <t>/kolam/:id</t>
-  </si>
-  <si>
     <t>menampilkan detail suatu kolam</t>
   </si>
   <si>
@@ -100,18 +97,12 @@
     <t>READ</t>
   </si>
   <si>
-    <t>/pangan/riwayat</t>
-  </si>
-  <si>
     <t>menampilkan seluruh riwayat pemberian pangan yang sudah terdaftar</t>
   </si>
   <si>
     <t>menambahkan / mendaftarkan riwayat pemberian pangan</t>
   </si>
   <si>
-    <t>/pangan/riwayat/:id</t>
-  </si>
-  <si>
     <t>menampilkan detail suatu riwayat pemberian pangan</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>menampilkan seluruh riwayat penggunaan user yang sudah terdaftar</t>
   </si>
   <si>
-    <t>/loguser/:id</t>
-  </si>
-  <si>
     <t>menampilkan detail suatu riwayat penggunaan user</t>
   </si>
   <si>
@@ -139,10 +127,22 @@
     <t>kolam</t>
   </si>
   <si>
-    <t>pemberian pangan</t>
-  </si>
-  <si>
     <t>loguser</t>
+  </si>
+  <si>
+    <t>/kolam/{kolam_id}</t>
+  </si>
+  <si>
+    <t>pemberian pakan</t>
+  </si>
+  <si>
+    <t>/riwayatpakan</t>
+  </si>
+  <si>
+    <t>/riwayatpakan/{logpakan_id}</t>
+  </si>
+  <si>
+    <t>/loguser/{loguser_id}</t>
   </si>
 </sst>
 </file>
@@ -220,19 +220,19 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -552,32 +552,32 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="85.5703125" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -589,80 +589,80 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -673,80 +673,80 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,35 +757,35 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>31</v>
+      <c r="E18" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>